<commit_message>
Agrego los cambios a cheatsheet.xls
</commit_message>
<xml_diff>
--- a/Git_y_Github_Lobos_Martin/Clase_6/Cheatsheet.xlsx
+++ b/Git_y_Github_Lobos_Martin/Clase_6/Cheatsheet.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lobma\Desktop\Clase 6 Intro\mochila_camada7\Git_y_Github_Lobos_Martin\Clase_6\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF488874-9F5E-4833-B310-C1B7E52D5E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,10 +24,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>Comandos mas utilizados</t>
+  </si>
+  <si>
+    <t>Funcion</t>
+  </si>
+  <si>
+    <t>git clone</t>
+  </si>
+  <si>
+    <t>clonar repo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git add . </t>
+  </si>
+  <si>
+    <t>adherir los archivos que realizamos cambios al stage</t>
+  </si>
+  <si>
+    <t>git commit - m "texto commit"</t>
+  </si>
+  <si>
+    <t>Agregar un commit para pushear</t>
+  </si>
+  <si>
+    <t>git push origin xxx</t>
+  </si>
+  <si>
+    <t>Subir los archivos a el repo remoto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git pull </t>
+  </si>
+  <si>
+    <r>
+      <t>Actulizar nuestros archivos</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> con el contenido del repo remoto</t>
+    </r>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +407,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="53.6640625" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Subiendo el Pdf (me olvide no me desapruebe pls)
</commit_message>
<xml_diff>
--- a/Git_y_Github_Lobos_Martin/Clase_6/Cheatsheet.xlsx
+++ b/Git_y_Github_Lobos_Martin/Clase_6/Cheatsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lobma\Desktop\Clase 6 Intro\mochila_camada7\Git_y_Github_Lobos_Martin\Clase_6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lobma\Desktop\Martín\CTD\Introducción a la Informatica\Clase 6 Intro\mochila_camada7\Git_y_Github_Lobos_Martin\Clase_6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF488874-9F5E-4833-B310-C1B7E52D5E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859C79B6-6E9A-4CEB-9F7A-04A1DE18D12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,7 +66,7 @@
     <r>
       <rPr>
         <u/>
-        <sz val="11"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -80,7 +80,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,7 +90,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="24"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -98,22 +105,28 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -121,13 +134,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,19 +438,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="53.6640625" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" customWidth="1"/>
+    <col min="2" max="2" width="73.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,48 +458,58 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>